<commit_message>
prueba 2 - estimación Pm
</commit_message>
<xml_diff>
--- a/Proyecto Interno/var-ipc/correlativa_ipc.xlsx
+++ b/Proyecto Interno/var-ipc/correlativa_ipc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portatil\Desktop\Least-cost-diets-and-affordability\Proyecto Interno\var-ipc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABC5F08-F897-4C77-B605-74E2BFCEC060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CDB55B-3CBD-4C2B-97DE-0D21F22CA241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC COICOP - IPC 2008" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="173">
   <si>
     <t>Arroz</t>
   </si>
@@ -226,9 +226,6 @@
     <t>011908</t>
   </si>
   <si>
-    <t>Leche en polvo para lactantes</t>
-  </si>
-  <si>
     <t>Otros alimentos precocidos y preparados: ajiaco, lenteja, frijol, lechona enlatada y similares</t>
   </si>
   <si>
@@ -409,9 +406,6 @@
     <t>011906</t>
   </si>
   <si>
-    <t>011911</t>
-  </si>
-  <si>
     <t>011999</t>
   </si>
   <si>
@@ -463,9 +457,6 @@
     <t>18102</t>
   </si>
   <si>
-    <t>17201</t>
-  </si>
-  <si>
     <t>Harina de maiz y otras harinas</t>
   </si>
   <si>
@@ -512,6 +503,42 @@
   </si>
   <si>
     <t>dane</t>
+  </si>
+  <si>
+    <t>011716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hortalizas y legumbres frescas </t>
+  </si>
+  <si>
+    <t>13104</t>
+  </si>
+  <si>
+    <t>13105</t>
+  </si>
+  <si>
+    <t>13201</t>
+  </si>
+  <si>
+    <t>13202</t>
+  </si>
+  <si>
+    <t>Revuelto verde</t>
+  </si>
+  <si>
+    <t>Fríjol</t>
+  </si>
+  <si>
+    <t>Arveja</t>
+  </si>
+  <si>
+    <t>011702</t>
+  </si>
+  <si>
+    <t>Legumbres secas</t>
+  </si>
+  <si>
+    <t>Otras hortalizas y legumbres secas</t>
   </si>
 </sst>
 </file>
@@ -565,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -609,8 +636,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -618,8 +657,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -645,13 +687,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3799410</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1028,38 +1070,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D266"/>
+  <dimension ref="A1:D269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="69" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="69" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="53.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="55.54296875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="55.5703125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>0</v>
@@ -1071,9 +1113,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -1085,9 +1127,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -1099,23 +1141,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="8">
         <v>11102</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="16"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="8">
         <v>11105</v>
       </c>
@@ -1123,23 +1165,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="8">
         <v>11102</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="16"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="8">
         <v>11105</v>
       </c>
@@ -1147,9 +1189,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -1161,33 +1203,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="8">
         <v>11102</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
-      <c r="B11" s="16"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="8">
         <v>11104</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
-      <c r="B12" s="16"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="8">
         <v>11202</v>
       </c>
@@ -1195,9 +1237,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
@@ -1209,9 +1251,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>10</v>
@@ -1223,9 +1265,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
@@ -1237,9 +1279,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>14</v>
@@ -1251,9 +1293,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>16</v>
@@ -1262,36 +1304,36 @@
         <v>15201</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="8">
         <v>16101</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
-      <c r="B19" s="16"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="8">
         <v>16201</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
@@ -1303,9 +1345,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>21</v>
@@ -1317,9 +1359,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>23</v>
@@ -1331,9 +1373,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>25</v>
@@ -1342,12 +1384,12 @@
         <v>17203</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>26</v>
@@ -1359,9 +1401,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>28</v>
@@ -1370,10 +1412,10 @@
         <v>17203</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
@@ -1387,9 +1429,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>32</v>
@@ -1397,19 +1439,19 @@
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>34</v>
@@ -1421,1315 +1463,1361 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="23">
+        <v>13203</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="8">
+        <v>13204</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="8">
-        <v>13204</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
+      <c r="B36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="8">
+        <v>12201</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="8">
-        <v>12201</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
+      <c r="B37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="8">
+        <v>12101</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="8">
-        <v>12101</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="7" t="s">
+      <c r="B38" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="8">
+        <v>12102</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="8">
-        <v>12102</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="7" t="s">
+      <c r="B39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="8">
+        <v>12103</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="8">
-        <v>12103</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="B41" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="8">
+        <v>18403</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="8">
+        <v>18404</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="8">
+        <v>18403</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="8">
+        <v>18403</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="8">
+        <v>18402</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="8">
+        <v>18301</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="8">
+        <v>18401</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="8">
+        <v>18404</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" s="8">
+        <v>18302</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="8">
-        <v>18403</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="17"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="8">
-        <v>18404</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="8">
-        <v>18403</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="8">
-        <v>18403</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="8">
-        <v>18402</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="8">
-        <v>18301</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="8">
-        <v>18401</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="7" t="s">
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="8">
-        <v>18404</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="8">
-        <v>13105</v>
-      </c>
-      <c r="D54" s="6" t="s">
+      <c r="B60" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="8">
+        <v>18201</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="8">
+        <v>18202</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="8">
+        <v>18503</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="17"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="8">
-        <v>18302</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="8">
-        <v>18201</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="8">
-        <v>18202</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="7" t="s">
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="7" t="s">
+      <c r="B65" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="8">
+        <v>18501</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C61" s="8">
-        <v>18503</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B62" s="4" t="s">
+      <c r="B66" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="8">
+        <v>18501</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="8">
-        <v>18501</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B63" s="4" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="8">
-        <v>18501</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="7" t="s">
+      <c r="B67" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="C67" s="8">
+        <v>18502</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="8">
-        <v>18502</v>
-      </c>
-      <c r="D64" s="1" t="s">
+    </row>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="9" t="s">
+      <c r="B68" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="2"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="2"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="2"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="7"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="7"/>
-    </row>
-    <row r="70" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="7"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="7"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="4"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="2"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
       <c r="B76" s="4"/>
       <c r="C76" s="7"/>
-      <c r="D76" s="6"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
       <c r="B78" s="4"/>
-      <c r="D78" s="6"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
       <c r="B79" s="4"/>
+      <c r="C79" s="7"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
       <c r="B80" s="4"/>
-      <c r="D80" s="6"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
       <c r="D81" s="6"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="D90" s="6"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="D91" s="6"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="D92" s="6"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="D93" s="6"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="D94" s="6"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="D95" s="6"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
       <c r="D97" s="6"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="4"/>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="4"/>
       <c r="D99" s="6"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="4"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="4"/>
       <c r="D101" s="6"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="4"/>
       <c r="D102" s="6"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="4"/>
       <c r="D103" s="6"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="4"/>
       <c r="D104" s="6"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="4"/>
       <c r="D105" s="6"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="4"/>
       <c r="D106" s="6"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="4"/>
       <c r="D107" s="6"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="4"/>
       <c r="D108" s="6"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="4"/>
       <c r="D109" s="6"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="4"/>
       <c r="D110" s="6"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="4"/>
       <c r="D111" s="6"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="4"/>
       <c r="D112" s="6"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="4"/>
       <c r="D113" s="6"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="4"/>
       <c r="D114" s="6"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="4"/>
       <c r="D115" s="6"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="4"/>
       <c r="D116" s="6"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="4"/>
       <c r="D117" s="6"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="4"/>
       <c r="D118" s="6"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="4"/>
       <c r="D119" s="6"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="4"/>
       <c r="D120" s="6"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="4"/>
       <c r="D121" s="6"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="4"/>
       <c r="D122" s="6"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="4"/>
       <c r="D123" s="6"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="4"/>
       <c r="D124" s="6"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="4"/>
       <c r="D125" s="6"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="4"/>
       <c r="D126" s="6"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="4"/>
       <c r="D127" s="6"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="4"/>
       <c r="D128" s="6"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="4"/>
       <c r="D129" s="6"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4"/>
       <c r="D130" s="6"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="4"/>
       <c r="D131" s="6"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="4"/>
       <c r="D132" s="6"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="4"/>
       <c r="D133" s="6"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="4"/>
       <c r="D134" s="6"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="4"/>
       <c r="D135" s="6"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="4"/>
       <c r="D136" s="6"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="4"/>
       <c r="D137" s="6"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="4"/>
       <c r="D138" s="6"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="4"/>
       <c r="D139" s="6"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="4"/>
       <c r="D140" s="6"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="4"/>
       <c r="D141" s="6"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="4"/>
       <c r="D142" s="6"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="4"/>
       <c r="D143" s="6"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="4"/>
       <c r="D144" s="6"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="4"/>
       <c r="D145" s="6"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="4"/>
       <c r="D146" s="6"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="4"/>
       <c r="D147" s="6"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="4"/>
       <c r="D148" s="6"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="4"/>
       <c r="D149" s="6"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="4"/>
       <c r="D150" s="6"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="4"/>
       <c r="D151" s="6"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="4"/>
       <c r="D152" s="6"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="4"/>
       <c r="D153" s="6"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="4"/>
       <c r="D154" s="6"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="4"/>
       <c r="D155" s="6"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="4"/>
       <c r="D156" s="6"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="4"/>
       <c r="D157" s="6"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="4"/>
       <c r="D158" s="6"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="4"/>
       <c r="D159" s="6"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="4"/>
       <c r="D160" s="6"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="4"/>
       <c r="D161" s="6"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="4"/>
       <c r="D162" s="6"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="4"/>
       <c r="D163" s="6"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="4"/>
       <c r="D164" s="6"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="4"/>
       <c r="D165" s="6"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="4"/>
       <c r="D166" s="6"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="4"/>
       <c r="D167" s="6"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="4"/>
       <c r="D168" s="6"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="4"/>
       <c r="D169" s="6"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="4"/>
       <c r="D170" s="6"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="4"/>
       <c r="D171" s="6"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="4"/>
       <c r="D172" s="6"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" s="4"/>
       <c r="D173" s="6"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="4"/>
       <c r="D174" s="6"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="4"/>
       <c r="D175" s="6"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="4"/>
       <c r="D176" s="6"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" s="4"/>
       <c r="D177" s="6"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" s="4"/>
       <c r="D178" s="6"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" s="4"/>
       <c r="D179" s="6"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
       <c r="D180" s="6"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" s="4"/>
       <c r="D181" s="6"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" s="4"/>
       <c r="D182" s="6"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" s="4"/>
       <c r="D183" s="6"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="4"/>
       <c r="D184" s="6"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="4"/>
       <c r="D185" s="6"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" s="4"/>
       <c r="D186" s="6"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" s="4"/>
       <c r="D187" s="6"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="4"/>
       <c r="D188" s="6"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="4"/>
       <c r="D189" s="6"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="4"/>
       <c r="D190" s="6"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" s="4"/>
       <c r="D191" s="6"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" s="4"/>
       <c r="D192" s="6"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" s="4"/>
       <c r="D193" s="6"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" s="4"/>
       <c r="D194" s="6"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="4"/>
       <c r="D195" s="6"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="4"/>
       <c r="D196" s="6"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" s="4"/>
       <c r="D197" s="6"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="4"/>
       <c r="D198" s="6"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="4"/>
       <c r="D199" s="6"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" s="4"/>
       <c r="D200" s="6"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="4"/>
       <c r="D201" s="6"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" s="4"/>
       <c r="D202" s="6"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="4"/>
       <c r="D203" s="6"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="4"/>
       <c r="D204" s="6"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="4"/>
       <c r="D205" s="6"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="4"/>
       <c r="D206" s="6"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" s="4"/>
       <c r="D207" s="6"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="4"/>
       <c r="D208" s="6"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B209" s="4"/>
       <c r="D209" s="6"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B210" s="4"/>
       <c r="D210" s="6"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B211" s="4"/>
       <c r="D211" s="6"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B212" s="4"/>
       <c r="D212" s="6"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B213" s="4"/>
       <c r="D213" s="6"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B214" s="4"/>
       <c r="D214" s="6"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B215" s="4"/>
       <c r="D215" s="6"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B216" s="4"/>
       <c r="D216" s="6"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B217" s="4"/>
       <c r="D217" s="6"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B218" s="4"/>
       <c r="D218" s="6"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B219" s="4"/>
       <c r="D219" s="6"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B220" s="4"/>
       <c r="D220" s="6"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="4"/>
       <c r="D221" s="6"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" s="4"/>
       <c r="D222" s="6"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B223" s="4"/>
       <c r="D223" s="6"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" s="4"/>
       <c r="D224" s="6"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="4"/>
       <c r="D225" s="6"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="4"/>
       <c r="D226" s="6"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" s="4"/>
       <c r="D227" s="6"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" s="4"/>
       <c r="D228" s="6"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="4"/>
       <c r="D229" s="6"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="4"/>
       <c r="D230" s="6"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="4"/>
       <c r="D231" s="6"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" s="4"/>
       <c r="D232" s="6"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" s="4"/>
       <c r="D233" s="6"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" s="4"/>
       <c r="D234" s="6"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="4"/>
       <c r="D235" s="6"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="4"/>
       <c r="D236" s="6"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B237" s="4"/>
       <c r="D237" s="6"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B238" s="4"/>
       <c r="D238" s="6"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" s="4"/>
       <c r="D239" s="6"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B240" s="4"/>
       <c r="D240" s="6"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="4"/>
       <c r="D241" s="6"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="4"/>
       <c r="D242" s="6"/>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="4"/>
       <c r="D243" s="6"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="4"/>
       <c r="D244" s="6"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="4"/>
       <c r="D245" s="6"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="4"/>
       <c r="D246" s="6"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="4"/>
       <c r="D247" s="6"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="4"/>
       <c r="D248" s="6"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="4"/>
       <c r="D249" s="6"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B250" s="4"/>
       <c r="D250" s="6"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" s="4"/>
       <c r="D251" s="6"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B252" s="4"/>
       <c r="D252" s="6"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B253" s="4"/>
       <c r="D253" s="6"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B254" s="4"/>
       <c r="D254" s="6"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B255" s="4"/>
       <c r="D255" s="6"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B256" s="4"/>
       <c r="D256" s="6"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B257" s="4"/>
       <c r="D257" s="6"/>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B258" s="4"/>
       <c r="D258" s="6"/>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B259" s="4"/>
       <c r="D259" s="6"/>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B260" s="4"/>
       <c r="D260" s="6"/>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B261" s="4"/>
       <c r="D261" s="6"/>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B262" s="4"/>
       <c r="D262" s="6"/>
     </row>
-    <row r="263" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B263" s="4"/>
       <c r="D263" s="6"/>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B264" s="4"/>
       <c r="D264" s="6"/>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B265" s="4"/>
       <c r="D265" s="6"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B266" s="4"/>
       <c r="D266" s="6"/>
     </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D267" s="6"/>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D268" s="6"/>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D269" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="19">
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C75:D75"/>
     <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
     <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C63:D63"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B10:B12"/>
@@ -2738,10 +2826,8 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A50:A51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>